<commit_message>
avoid having any 'extra' blank rows after all the data has been read.
</commit_message>
<xml_diff>
--- a/src/test/resources/repro.xlsx
+++ b/src/test/resources/repro.xlsx
@@ -3,13 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10908"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F65F40-C514-F849-A007-289618291B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FD0CC3-6711-9E4D-8020-4C85CB4D9573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" tabRatio="903" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" tabRatio="903" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BadRow" sheetId="7" r:id="rId1"/>
     <sheet name="WithUnicode" sheetId="8" r:id="rId2"/>
+    <sheet name="ExtraBlankRowsAfterData" sheetId="9" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>aaa</t>
   </si>
@@ -51,17 +53,31 @@
   <si>
     <t>déjà vu</t>
   </si>
+  <si>
+    <t>aa11</t>
+  </si>
+  <si>
+    <t>bb22</t>
+  </si>
+  <si>
+    <t>cc33</t>
+  </si>
+  <si>
+    <t>dd44</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="#.00,"/>
+    <numFmt numFmtId="170" formatCode="0.0?"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +109,13 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -119,11 +142,14 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="5" builtinId="3"/>
@@ -628,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7AF7C1-D6A4-2043-83F8-BF6805DD6E95}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
@@ -652,6 +678,83 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C08A3FB-3150-4347-8F13-54122C7BD011}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4034CC2-F6C0-BC41-93FE-1AC45C535523}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1693,6 +1796,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>AssetEditForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <APDescription xmlns="4873beb7-5857-4685-be1f-d57550cc96cc" xsi:nil="true"/>
@@ -1827,15 +1939,6 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>AssetEditForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A47D5F50-61BF-43FC-88EE-AB79032B7FF4}">
   <ds:schemaRefs>
@@ -1855,6 +1958,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F99384FD-992A-4406-BDB3-5B1113759664}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7868694D-5EA1-4970-B8F2-C7BE7A5B832E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -1868,12 +1979,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F99384FD-992A-4406-BDB3-5B1113759664}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>